<commit_message>
Minor part list edits
</commit_message>
<xml_diff>
--- a/BOM/ID Lists.xlsx
+++ b/BOM/ID Lists.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2790343D-308A-4040-80E0-2800B079B204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87187C3E-349E-4FEB-AB87-F9315655B9B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{2BA3904D-48D5-4484-9C88-BD860323DFB0}"/>
+    <workbookView xWindow="37464" yWindow="4332" windowWidth="17196" windowHeight="10356" activeTab="1" xr2:uid="{2BA3904D-48D5-4484-9C88-BD860323DFB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Electrical IDs" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="492">
   <si>
     <t>Short Name</t>
   </si>
@@ -514,30 +514,15 @@
     <t>PSU DC to MCU, pair 3</t>
   </si>
   <si>
-    <t>DC24-B1</t>
-  </si>
-  <si>
     <t>DC24-A3</t>
   </si>
   <si>
     <t>PSU DC to 5V Buck</t>
   </si>
   <si>
-    <t>EARTH-A</t>
-  </si>
-  <si>
     <t>EARTH</t>
   </si>
   <si>
-    <t>AC Earth to PSU Earth</t>
-  </si>
-  <si>
-    <t>EARTH-B</t>
-  </si>
-  <si>
-    <t>PSU Earth to Frame</t>
-  </si>
-  <si>
     <t>TB-A</t>
   </si>
   <si>
@@ -1511,6 +1496,24 @@
   </si>
   <si>
     <t>Bare</t>
+  </si>
+  <si>
+    <t>GND-A</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t>GND-B</t>
+  </si>
+  <si>
+    <t>PSU Ground to Frame</t>
+  </si>
+  <si>
+    <t>AC GND to PSU GND</t>
+  </si>
+  <si>
+    <t>DC24-B</t>
   </si>
 </sst>
 </file>
@@ -2451,7 +2454,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -2459,13 +2462,13 @@
         <v>146</v>
       </c>
       <c r="B35" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C35" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="D35" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -2473,38 +2476,38 @@
         <v>153</v>
       </c>
       <c r="B36" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C36" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B37" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C37" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="D37" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="B38" t="s">
+        <v>477</v>
+      </c>
+      <c r="C38" t="s">
         <v>482</v>
       </c>
-      <c r="C38" t="s">
-        <v>487</v>
-      </c>
       <c r="D38" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
     </row>
   </sheetData>
@@ -2520,8 +2523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{220CAEEC-A537-49E7-8CB6-74590B623C46}">
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2552,7 +2555,7 @@
         <v>117</v>
       </c>
       <c r="F1" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="G1" t="s">
         <v>99</v>
@@ -2566,7 +2569,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
@@ -2585,7 +2588,7 @@
         <v>70</v>
       </c>
       <c r="G2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="H2" t="s">
         <v>148</v>
@@ -2623,7 +2626,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B4" t="s">
         <v>146</v>
@@ -2653,7 +2656,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B5" t="s">
         <v>146</v>
@@ -2743,7 +2746,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B8" t="s">
         <v>153</v>
@@ -2773,10 +2776,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>161</v>
+        <v>486</v>
       </c>
       <c r="B9" t="s">
-        <v>162</v>
+        <v>487</v>
       </c>
       <c r="C9">
         <v>16</v>
@@ -2798,15 +2801,15 @@
         <v>148</v>
       </c>
       <c r="I9" t="s">
-        <v>163</v>
+        <v>490</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>164</v>
+        <v>488</v>
       </c>
       <c r="B10" t="s">
-        <v>162</v>
+        <v>487</v>
       </c>
       <c r="C10">
         <v>16</v>
@@ -2828,7 +2831,7 @@
         <v>148</v>
       </c>
       <c r="I10" t="s">
-        <v>165</v>
+        <v>489</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2852,10 +2855,10 @@
         <v>110</v>
       </c>
       <c r="G11" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="H11" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2879,15 +2882,15 @@
         <v>300</v>
       </c>
       <c r="G12" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="H12" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>158</v>
+        <v>491</v>
       </c>
       <c r="B13" t="s">
         <v>153</v>
@@ -2909,10 +2912,10 @@
         <v>148</v>
       </c>
       <c r="H13" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="I13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2936,10 +2939,10 @@
         <v>90</v>
       </c>
       <c r="G14" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="H14" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2963,10 +2966,10 @@
         <v>300</v>
       </c>
       <c r="G15" t="s">
+        <v>202</v>
+      </c>
+      <c r="H15" t="s">
         <v>207</v>
-      </c>
-      <c r="H15" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2990,10 +2993,10 @@
         <v>90</v>
       </c>
       <c r="G16" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="H16" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -3017,10 +3020,10 @@
         <v>300</v>
       </c>
       <c r="G17" t="s">
+        <v>202</v>
+      </c>
+      <c r="H17" t="s">
         <v>207</v>
-      </c>
-      <c r="H17" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -3044,10 +3047,10 @@
         <v>80</v>
       </c>
       <c r="G18" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="H18" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -3071,10 +3074,10 @@
         <v>300</v>
       </c>
       <c r="G19" t="s">
+        <v>202</v>
+      </c>
+      <c r="H19" t="s">
         <v>207</v>
-      </c>
-      <c r="H19" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -3101,10 +3104,10 @@
         <v>144</v>
       </c>
       <c r="H20" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="I20" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -3128,10 +3131,10 @@
         <v>750</v>
       </c>
       <c r="G21" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="H21" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -3155,10 +3158,10 @@
         <v>140</v>
       </c>
       <c r="G22" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="H22" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -3182,10 +3185,10 @@
         <v>600</v>
       </c>
       <c r="G23" t="s">
+        <v>204</v>
+      </c>
+      <c r="H23" t="s">
         <v>209</v>
-      </c>
-      <c r="H23" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -3209,10 +3212,10 @@
         <v>20</v>
       </c>
       <c r="G24" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="H24" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="I24" t="s">
         <v>125</v>
@@ -3239,10 +3242,10 @@
         <v>135</v>
       </c>
       <c r="G25" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="H25" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -3266,10 +3269,10 @@
         <v>240</v>
       </c>
       <c r="G26" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="H26" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -3293,13 +3296,13 @@
         <v>15</v>
       </c>
       <c r="G27" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="H27" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="I27" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -3323,10 +3326,10 @@
         <v>240</v>
       </c>
       <c r="G28" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="H28" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -3350,10 +3353,10 @@
         <v>240</v>
       </c>
       <c r="G29" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="H29" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -3377,13 +3380,13 @@
         <v>15</v>
       </c>
       <c r="G30" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="H30" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="I30" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -3407,13 +3410,13 @@
         <v>240</v>
       </c>
       <c r="G31" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="H31" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="I31" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -3437,10 +3440,10 @@
         <v>330</v>
       </c>
       <c r="G32" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="H32" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -3464,13 +3467,13 @@
         <v>15</v>
       </c>
       <c r="G33" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="H33" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="I33" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -3494,10 +3497,10 @@
         <v>105</v>
       </c>
       <c r="G34" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="H34" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -3521,10 +3524,10 @@
         <v>270</v>
       </c>
       <c r="G35" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="H35" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -3548,10 +3551,10 @@
         <v>90</v>
       </c>
       <c r="G36" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="H36" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -3575,10 +3578,10 @@
         <v>315</v>
       </c>
       <c r="G37" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="H37" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -3602,10 +3605,10 @@
         <v>195</v>
       </c>
       <c r="G38" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="H38" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -3629,10 +3632,10 @@
         <v>225</v>
       </c>
       <c r="G39" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="H39" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -3656,10 +3659,10 @@
         <v>90</v>
       </c>
       <c r="G40" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="H40" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -3683,10 +3686,10 @@
         <v>225</v>
       </c>
       <c r="G41" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="H41" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -3710,10 +3713,10 @@
         <v>280</v>
       </c>
       <c r="G42" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="H42" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -3737,10 +3740,10 @@
         <v>400</v>
       </c>
       <c r="G43" t="s">
+        <v>204</v>
+      </c>
+      <c r="H43" t="s">
         <v>209</v>
-      </c>
-      <c r="H43" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -3764,10 +3767,10 @@
         <v>280</v>
       </c>
       <c r="G44" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="H44" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -3791,10 +3794,10 @@
         <v>400</v>
       </c>
       <c r="G45" t="s">
+        <v>204</v>
+      </c>
+      <c r="H45" t="s">
         <v>209</v>
-      </c>
-      <c r="H45" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -3818,10 +3821,10 @@
         <v>120</v>
       </c>
       <c r="G46" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="H46" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="I46" t="s">
         <v>125</v>
@@ -3848,10 +3851,10 @@
         <v>160</v>
       </c>
       <c r="G47" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="H47" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="I47" t="s">
         <v>125</v>
@@ -3859,7 +3862,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B48" t="s">
         <v>24</v>
@@ -3878,15 +3881,15 @@
         <v>120</v>
       </c>
       <c r="G48" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="H48" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B49" t="s">
         <v>31</v>
@@ -3905,15 +3908,15 @@
         <v>120</v>
       </c>
       <c r="G49" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="H49" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B50" t="s">
         <v>31</v>
@@ -3932,15 +3935,15 @@
         <v>70</v>
       </c>
       <c r="G50" t="s">
+        <v>202</v>
+      </c>
+      <c r="H50" t="s">
         <v>207</v>
-      </c>
-      <c r="H50" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B51" t="s">
         <v>41</v>
@@ -3962,12 +3965,12 @@
         <v>143</v>
       </c>
       <c r="H51" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B52" t="s">
         <v>33</v>
@@ -3986,15 +3989,15 @@
         <v>120</v>
       </c>
       <c r="G52" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="H52" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B53" t="s">
         <v>33</v>
@@ -4013,15 +4016,15 @@
         <v>140</v>
       </c>
       <c r="G53" t="s">
+        <v>202</v>
+      </c>
+      <c r="H53" t="s">
         <v>207</v>
-      </c>
-      <c r="H53" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B54" t="s">
         <v>33</v>
@@ -4040,15 +4043,15 @@
         <v>120</v>
       </c>
       <c r="G54" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="H54" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B55" t="s">
         <v>33</v>
@@ -4067,15 +4070,15 @@
         <v>140</v>
       </c>
       <c r="G55" t="s">
+        <v>202</v>
+      </c>
+      <c r="H55" t="s">
         <v>207</v>
-      </c>
-      <c r="H55" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B56" t="s">
         <v>60</v>
@@ -4094,18 +4097,18 @@
         <v>170</v>
       </c>
       <c r="G56" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="H56" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="I56" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B57" t="s">
         <v>60</v>
@@ -4124,18 +4127,18 @@
         <v>85</v>
       </c>
       <c r="G57" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="H57" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="I57" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B58" t="s">
         <v>60</v>
@@ -4154,7 +4157,7 @@
         <v>170</v>
       </c>
       <c r="G58" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="H58" t="s">
         <v>148</v>
@@ -4181,10 +4184,10 @@
         <v>30</v>
       </c>
       <c r="G59" t="s">
+        <v>201</v>
+      </c>
+      <c r="H59" t="s">
         <v>206</v>
-      </c>
-      <c r="H59" t="s">
-        <v>211</v>
       </c>
       <c r="I59" t="s">
         <v>123</v>
@@ -4215,10 +4218,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C1" t="s">
         <v>90</v>
@@ -4232,47 +4235,47 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B2" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C2" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D2">
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B3" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D3">
         <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B4" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D4">
         <v>100</v>
@@ -4280,36 +4283,36 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B5" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C5" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D5">
         <v>100</v>
       </c>
       <c r="E5" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B6" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C6" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="D6">
         <v>60</v>
       </c>
       <c r="E6" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -4324,8 +4327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E1B02D3-B4BD-4CA5-AFCD-0AF29CD03E0E}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4338,27 +4341,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C1" t="s">
         <v>90</v>
       </c>
       <c r="D1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B2" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C2" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="D2">
         <v>11</v>
@@ -4366,13 +4369,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B3" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C3" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="D3">
         <v>11</v>
@@ -4380,13 +4383,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B4" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C4" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D4">
         <v>6</v>
@@ -4394,13 +4397,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B5" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C5" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D5">
         <v>6</v>
@@ -4408,13 +4411,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B6" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C6" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D6">
         <v>11</v>
@@ -4422,13 +4425,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B7" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C7" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D7">
         <v>10</v>
@@ -4436,13 +4439,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B8" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C8" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D8">
         <v>10</v>
@@ -4450,13 +4453,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B9" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C9" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D9">
         <v>8</v>
@@ -4464,13 +4467,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B10" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C10" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D10">
         <v>8</v>
@@ -4478,13 +4481,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B11" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C11" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D11">
         <v>6</v>
@@ -4492,13 +4495,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B12" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C12" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D12">
         <v>9</v>
@@ -4506,13 +4509,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B13" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="C13" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D13">
         <v>14</v>
@@ -4520,13 +4523,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B14" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="C14" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D14">
         <v>14</v>
@@ -4534,13 +4537,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="B15" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="C15" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -4548,13 +4551,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>255</v>
+      </c>
+      <c r="B16" t="s">
+        <v>258</v>
+      </c>
+      <c r="C16" t="s">
         <v>260</v>
-      </c>
-      <c r="B16" t="s">
-        <v>263</v>
-      </c>
-      <c r="C16" t="s">
-        <v>265</v>
       </c>
       <c r="D16">
         <v>4</v>
@@ -4562,13 +4565,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>256</v>
+      </c>
+      <c r="B17" t="s">
+        <v>259</v>
+      </c>
+      <c r="C17" t="s">
         <v>261</v>
-      </c>
-      <c r="B17" t="s">
-        <v>264</v>
-      </c>
-      <c r="C17" t="s">
-        <v>266</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -4576,13 +4579,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="B18" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C18" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D18">
         <v>2</v>
@@ -4590,13 +4593,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="B19" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C19" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D19">
         <v>4</v>
@@ -4604,13 +4607,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B20" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C20" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D20">
         <v>4</v>
@@ -4621,10 +4624,10 @@
         <v>97</v>
       </c>
       <c r="B21" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C21" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D21">
         <v>6</v>
@@ -4635,10 +4638,10 @@
         <v>93</v>
       </c>
       <c r="B22" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="C22" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D22">
         <v>8</v>
@@ -4649,10 +4652,10 @@
         <v>92</v>
       </c>
       <c r="B23" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C23" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="D23">
         <v>14</v>
@@ -4660,13 +4663,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B24" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C24" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="D24">
         <v>11</v>
@@ -4674,13 +4677,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B25" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C25" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="D25">
         <v>4</v>
@@ -4688,13 +4691,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B26" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C26" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D26">
         <v>6</v>
@@ -4702,13 +4705,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B27" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="C27" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D27">
         <v>8</v>
@@ -4716,13 +4719,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B28" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C28" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="D28">
         <v>11</v>
@@ -4730,13 +4733,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B29" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C29" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="D29">
         <v>11</v>
@@ -4744,13 +4747,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B30" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C30" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="D30">
         <v>4</v>
@@ -4758,13 +4761,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B31" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C31" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D31">
         <v>7</v>
@@ -4772,13 +4775,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="B32" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C32" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D32">
         <v>5</v>
@@ -4786,13 +4789,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B33" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="C33" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="D33">
         <v>15</v>
@@ -4800,13 +4803,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B34" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="C34" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="D34">
         <v>14</v>
@@ -4814,13 +4817,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B35" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="C35" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D35">
         <v>10</v>
@@ -4852,33 +4855,33 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="B1" t="s">
         <v>90</v>
       </c>
       <c r="C1" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="E1" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="F1" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="C2" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -4893,13 +4896,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="C3" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -4914,13 +4917,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="C4" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -4935,13 +4938,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="C5" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -4956,13 +4959,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="C6" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -4977,13 +4980,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="C7" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -4998,13 +5001,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="C8" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -5019,13 +5022,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="C9" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -5040,13 +5043,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="C10" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -5061,13 +5064,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="C11" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D11">
         <v>4</v>
@@ -5082,13 +5085,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="C12" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -5103,13 +5106,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="C13" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -5124,13 +5127,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="C14" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -5145,13 +5148,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="C15" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D15">
         <v>3</v>
@@ -5166,13 +5169,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="C16" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -5187,13 +5190,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="C17" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -5208,13 +5211,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="C18" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -5229,13 +5232,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="C19" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -5250,13 +5253,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="C20" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -5271,13 +5274,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="C21" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -5292,13 +5295,13 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="C22" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D22">
         <v>2</v>
@@ -5313,13 +5316,13 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="C23" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D23">
         <v>2</v>
@@ -5334,13 +5337,13 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="C24" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -5355,13 +5358,13 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="C25" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -5376,13 +5379,13 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="C26" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D26">
         <v>2</v>
@@ -5397,13 +5400,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="C27" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D27">
         <v>2</v>
@@ -5418,13 +5421,13 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="C28" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -5439,13 +5442,13 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="C29" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -5460,13 +5463,13 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="C30" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -5481,13 +5484,13 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="C31" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D31">
         <v>3</v>
@@ -5502,13 +5505,13 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="C32" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D32">
         <v>6</v>
@@ -5523,13 +5526,13 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="C33" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D33">
         <v>4</v>
@@ -5544,13 +5547,13 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="C34" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D34">
         <v>8</v>
@@ -5565,13 +5568,13 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="C35" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -5586,13 +5589,13 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="C36" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -5607,13 +5610,13 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="C37" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D37">
         <v>6</v>
@@ -5628,13 +5631,13 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="C38" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -5649,13 +5652,13 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="C39" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D39">
         <v>2</v>
@@ -5670,13 +5673,13 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="C40" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -5691,13 +5694,13 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="C41" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D41">
         <v>2</v>
@@ -5712,13 +5715,13 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="C42" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -5733,13 +5736,13 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="C43" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D43">
         <v>2</v>
@@ -5754,13 +5757,13 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="C44" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -5775,13 +5778,13 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="C45" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -5796,13 +5799,13 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="C46" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -5817,13 +5820,13 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="C47" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D47">
         <v>4</v>
@@ -5838,13 +5841,13 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="C48" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D48">
         <v>4</v>
@@ -5859,13 +5862,13 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="C49" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D49">
         <v>2</v>
@@ -5880,13 +5883,13 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="C50" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D50">
         <v>2</v>
@@ -5901,13 +5904,13 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="C51" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -5922,13 +5925,13 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="C52" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D52">
         <v>2</v>
@@ -5943,13 +5946,13 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="C53" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D53">
         <v>2</v>
@@ -5964,13 +5967,13 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="C54" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -5985,13 +5988,13 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="C55" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -6006,13 +6009,13 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="C56" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -6027,13 +6030,13 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="C57" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -6048,13 +6051,13 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="C58" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -6069,13 +6072,13 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="C59" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -6090,13 +6093,13 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="C60" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D60">
         <v>1</v>
@@ -6111,13 +6114,13 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="C61" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -6132,13 +6135,13 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="C62" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -6153,13 +6156,13 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="C63" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -6174,13 +6177,13 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="C64" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -6195,13 +6198,13 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="C65" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -6216,13 +6219,13 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="C66" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D66">
         <v>2</v>
@@ -6237,13 +6240,13 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="C67" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D67">
         <v>4</v>
@@ -6258,13 +6261,13 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="C68" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -6279,13 +6282,13 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="C69" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D69">
         <v>2</v>
@@ -6300,13 +6303,13 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="C70" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D70">
         <v>2</v>
@@ -6321,13 +6324,13 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="C71" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -6342,13 +6345,13 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="C72" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D72">
         <v>2</v>
@@ -6363,13 +6366,13 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="C73" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D73">
         <v>2</v>
@@ -6384,13 +6387,13 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="C74" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -6405,13 +6408,13 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="C75" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D75">
         <v>7</v>
@@ -6426,13 +6429,13 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="C76" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D76">
         <v>2</v>
@@ -6447,13 +6450,13 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="C77" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -6468,13 +6471,13 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="C78" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -6489,13 +6492,13 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="C79" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="D79">
         <v>0</v>
@@ -6510,13 +6513,13 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C80" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -6531,13 +6534,13 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="C81" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -6552,13 +6555,13 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="C82" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -6573,13 +6576,13 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="C83" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D83">
         <v>0</v>
@@ -6594,13 +6597,13 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="C84" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -6615,13 +6618,13 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="C85" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="D85">
         <v>0</v>
@@ -6636,13 +6639,13 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="C86" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -6657,13 +6660,13 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="C87" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -6678,13 +6681,13 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="C88" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D88">
         <v>10</v>
@@ -6699,13 +6702,13 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="C89" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D89">
         <v>0</v>
@@ -6720,13 +6723,13 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="C90" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D90">
         <v>0</v>
@@ -6741,13 +6744,13 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="C91" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="D91">
         <v>0</v>
@@ -6762,13 +6765,13 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="C92" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="D92">
         <v>0</v>
@@ -6783,13 +6786,13 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="C93" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D93">
         <v>0</v>
@@ -6804,13 +6807,13 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="C94" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D94">
         <v>0</v>
@@ -6825,13 +6828,13 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="C95" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D95">
         <v>0</v>
@@ -6846,13 +6849,13 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="C96" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D96">
         <v>1</v>
@@ -6867,7 +6870,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="B97" s="6"/>
       <c r="F97">

</xml_diff>